<commit_message>
Add some folders and modify readme.md
</commit_message>
<xml_diff>
--- a/document/All/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
+++ b/document/All/Chi tiet tra no-Hoang Ngoc Anh 26.08.2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="645" windowWidth="15570" windowHeight="6825" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="705" windowWidth="15570" windowHeight="6765" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Du no TD" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,14 @@
   <definedNames>
     <definedName name="FU">[1]FU!#REF!</definedName>
     <definedName name="HK">[2]HK!$D$2:$D$19</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>MSSV</t>
   </si>
@@ -265,12 +266,15 @@
   </si>
   <si>
     <t>SE61099</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="12">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -285,7 +289,7 @@
     <numFmt numFmtId="172" formatCode="_-* #,##0.0\ _₫_-;\-* #,##0.0\ _₫_-;_-* &quot;-&quot;?\ _₫_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -825,8 +829,36 @@
     <cellStyle name="Normal 7 2" xfId="14"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -836,7 +868,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="DS1(101 SV cho TN)"/>
@@ -867,7 +899,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FU"/>
@@ -1057,6 +1089,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1091,6 +1124,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1266,14 +1300,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.75" bestFit="1" customWidth="1"/>
@@ -1292,7 +1326,7 @@
     <col min="18" max="18" width="11.125" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1346,7 @@
       <c r="K1" s="42"/>
       <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>79</v>
       </c>
@@ -1335,7 +1369,7 @@
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="48"/>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
@@ -1365,7 +1399,7 @@
         <v>1.7808219178082192E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="26" customFormat="1">
+    <row r="4" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="87" t="s">
         <v>2</v>
       </c>
@@ -1409,7 +1443,7 @@
       </c>
       <c r="R4" s="35"/>
     </row>
-    <row r="5" spans="1:18" s="26" customFormat="1">
+    <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="88"/>
       <c r="B5" s="84"/>
       <c r="C5" s="39" t="s">
@@ -1453,7 +1487,7 @@
       </c>
       <c r="R5" s="35"/>
     </row>
-    <row r="6" spans="1:18" s="28" customFormat="1">
+    <row r="6" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>40798</v>
       </c>
@@ -1484,7 +1518,7 @@
       <c r="M6" s="24"/>
       <c r="R6" s="36"/>
     </row>
-    <row r="7" spans="1:18" s="28" customFormat="1">
+    <row r="7" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>40798</v>
       </c>
@@ -1521,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1">
+    <row r="8" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>68</v>
       </c>
@@ -1579,7 +1613,7 @@
         <v>1507631.5410958903</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="26" customFormat="1">
+    <row r="9" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="s">
         <v>69</v>
       </c>
@@ -1637,7 +1671,7 @@
         <v>1431391.9520547944</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="26" customFormat="1">
+    <row r="10" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>41025</v>
       </c>
@@ -1675,7 +1709,7 @@
         <v>41025</v>
       </c>
       <c r="N10" s="26">
-        <f t="shared" ref="N9:N11" si="7">$N$5-M10</f>
+        <f t="shared" ref="N10:N11" si="7">$N$5-M10</f>
         <v>127</v>
       </c>
       <c r="O10" s="26">
@@ -1695,7 +1729,7 @@
         <v>3187450.8630136987</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="26" customFormat="1">
+    <row r="11" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>41151</v>
       </c>
@@ -1753,7 +1787,7 @@
         <v>2632974.9178082189</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="26" customFormat="1">
+    <row r="12" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>71</v>
       </c>
@@ -1807,7 +1841,7 @@
         <v>2291928.2054794519</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="26" customFormat="1">
+    <row r="13" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>72</v>
       </c>
@@ -1861,7 +1895,7 @@
         <v>1948469.1780821914</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="26" customFormat="1">
+    <row r="14" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>41512</v>
       </c>
@@ -1914,7 +1948,7 @@
         <v>1637936.9178082191</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="26" customFormat="1">
+    <row r="15" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
         <v>73</v>
       </c>
@@ -1963,7 +1997,7 @@
         <v>1350158.8356164382</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="26" customFormat="1">
+    <row r="16" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
         <v>74</v>
       </c>
@@ -2012,7 +2046,7 @@
         <v>1055186.3013698629</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="26" customFormat="1">
+    <row r="17" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>75</v>
       </c>
@@ -2061,7 +2095,7 @@
         <v>757815.61643835611</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="26" customFormat="1">
+    <row r="18" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="75" t="s">
         <v>76</v>
       </c>
@@ -2106,7 +2140,7 @@
         <v>507128.93150684936</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="50" customFormat="1">
+    <row r="19" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="82" t="s">
         <v>16</v>
       </c>
@@ -2152,7 +2186,7 @@
       <c r="Q19" s="26"/>
       <c r="R19" s="35"/>
     </row>
-    <row r="20" spans="1:18" s="50" customFormat="1">
+    <row r="20" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -2175,7 +2209,7 @@
         <v>18308073.260273971</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="56"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -2191,13 +2225,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="35"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N22" s="25"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N23" s="25"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="54" t="s">
         <v>19</v>
       </c>
@@ -2208,10 +2242,13 @@
       <c r="D24" s="62" t="s">
         <v>77</v>
       </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="N24" s="25"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="54" t="s">
         <v>18</v>
       </c>
@@ -2222,9 +2259,12 @@
       <c r="D25" s="62" t="s">
         <v>77</v>
       </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
       <c r="N25" s="25"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="54" t="s">
         <v>17</v>
       </c>
@@ -2235,10 +2275,13 @@
       <c r="D26" s="62" t="s">
         <v>77</v>
       </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="N26" s="25"/>
     </row>
-    <row r="27" spans="1:18" hidden="1">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="54" t="s">
         <v>51</v>
       </c>
@@ -2250,7 +2293,7 @@
       </c>
       <c r="N27" s="25"/>
     </row>
-    <row r="28" spans="1:18" hidden="1">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="54" t="s">
         <v>53</v>
       </c>
@@ -2263,7 +2306,7 @@
       </c>
       <c r="N28" s="25"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="60" t="s">
         <v>54</v>
       </c>
@@ -2274,9 +2317,12 @@
       <c r="D29" s="62" t="s">
         <v>77</v>
       </c>
+      <c r="E29" t="s">
+        <v>80</v>
+      </c>
       <c r="N29" s="25"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="60" t="s">
         <v>18</v>
       </c>
@@ -2287,7 +2333,7 @@
       <c r="D30" s="62"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="60" t="s">
         <v>55</v>
       </c>
@@ -2298,7 +2344,7 @@
       <c r="D31" s="62"/>
       <c r="F31" s="37"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="60" t="s">
         <v>56</v>
       </c>
@@ -2309,7 +2355,7 @@
       <c r="D32" s="63"/>
       <c r="F32" s="37"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="60" t="s">
         <v>57</v>
       </c>
@@ -2322,10 +2368,10 @@
       </c>
       <c r="F33" s="37"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F34" s="37"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="93" t="s">
         <v>3</v>
       </c>
@@ -2338,7 +2384,7 @@
       </c>
       <c r="F35" s="95"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="77" t="s">
         <v>19</v>
       </c>
@@ -2352,7 +2398,7 @@
       </c>
       <c r="F36" s="80"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="77" t="s">
         <v>18</v>
       </c>
@@ -2366,7 +2412,7 @@
       </c>
       <c r="F37" s="80"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="77" t="s">
         <v>17</v>
       </c>
@@ -2380,7 +2426,7 @@
       </c>
       <c r="F38" s="80"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="77" t="s">
         <v>18</v>
       </c>
@@ -2394,7 +2440,7 @@
       </c>
       <c r="F39" s="80"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="77" t="s">
         <v>60</v>
       </c>
@@ -2408,7 +2454,7 @@
       </c>
       <c r="F40" s="80"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="77" t="s">
         <v>58</v>
       </c>
@@ -2422,7 +2468,7 @@
       </c>
       <c r="F41" s="80"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="77" t="s">
         <v>61</v>
       </c>
@@ -2436,7 +2482,7 @@
       </c>
       <c r="F42" s="80"/>
     </row>
-    <row r="43" spans="2:6" ht="37.5" customHeight="1">
+    <row r="43" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="81" t="s">
         <v>62</v>
       </c>
@@ -2489,14 +2535,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="3" customWidth="1"/>
@@ -2510,7 +2556,7 @@
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.75" customHeight="1">
+    <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
         <v>41</v>
       </c>
@@ -2523,7 +2569,7 @@
       <c r="H1" s="96"/>
       <c r="I1" s="96"/>
     </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2540,7 +2586,7 @@
       </c>
       <c r="H3" s="38"/>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -2559,7 +2605,7 @@
       </c>
       <c r="H4" s="38"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5" customHeight="1">
+    <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -2573,7 +2619,7 @@
       <c r="D5" s="9"/>
       <c r="H5" s="38"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5" customHeight="1">
+    <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -2587,7 +2633,7 @@
       <c r="D6" s="9"/>
       <c r="H6" s="38"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2609,7 +2655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -2620,10 +2666,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1">
+    <row r="10" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>33</v>
       </c>
@@ -2652,7 +2698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1">
+    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="57">
         <v>1</v>
       </c>
@@ -2684,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1">
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -2716,7 +2762,7 @@
         <v>-298</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1">
+    <row r="13" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -2748,7 +2794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1">
+    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="57">
         <v>4</v>
       </c>
@@ -2780,7 +2826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1">
+    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>5</v>
       </c>
@@ -2812,7 +2858,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="57">
         <v>6</v>
       </c>
@@ -2844,7 +2890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>7</v>
       </c>
@@ -2877,7 +2923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>8</v>
       </c>
@@ -2910,7 +2956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="57">
         <v>9</v>
       </c>
@@ -2943,7 +2989,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>10</v>
       </c>
@@ -2976,7 +3022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="57">
         <v>11</v>
       </c>
@@ -3009,7 +3055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>12</v>
       </c>
@@ -3044,7 +3090,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>13</v>
       </c>
@@ -3077,7 +3123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="57">
         <v>14</v>
       </c>
@@ -3110,7 +3156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>15</v>
       </c>
@@ -3143,7 +3189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="57">
         <v>16</v>
       </c>
@@ -3176,7 +3222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>17</v>
       </c>
@@ -3209,7 +3255,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>18</v>
       </c>
@@ -3242,7 +3288,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="57">
         <v>19</v>
       </c>
@@ -3275,7 +3321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>20</v>
       </c>
@@ -3308,7 +3354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="57">
         <v>21</v>
       </c>
@@ -3341,7 +3387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>22</v>
       </c>
@@ -3374,7 +3420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>23</v>
       </c>
@@ -3407,7 +3453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="57">
         <v>24</v>
       </c>
@@ -3442,7 +3488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>25</v>
       </c>
@@ -3474,7 +3520,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="57">
         <v>26</v>
       </c>
@@ -3506,7 +3552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>27</v>
       </c>
@@ -3538,7 +3584,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>28</v>
       </c>
@@ -3570,7 +3616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="57">
         <v>29</v>
       </c>
@@ -3602,7 +3648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>30</v>
       </c>
@@ -3634,7 +3680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="57">
         <v>31</v>
       </c>
@@ -3666,7 +3712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>32</v>
       </c>
@@ -3698,7 +3744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>33</v>
       </c>
@@ -3730,7 +3776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="57">
         <v>34</v>
       </c>
@@ -3762,7 +3808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>35</v>
       </c>
@@ -3794,7 +3840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="57">
         <v>36</v>
       </c>
@@ -3829,7 +3875,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>37</v>
       </c>
@@ -3861,7 +3907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>38</v>
       </c>
@@ -3893,7 +3939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="57">
         <v>39</v>
       </c>
@@ -3925,7 +3971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>40</v>
       </c>
@@ -3957,7 +4003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="57">
         <v>41</v>
       </c>
@@ -3989,7 +4035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>42</v>
       </c>
@@ -4021,7 +4067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>43</v>
       </c>
@@ -4053,7 +4099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="57">
         <v>44</v>
       </c>
@@ -4085,7 +4131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>45</v>
       </c>
@@ -4117,7 +4163,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="57">
         <v>46</v>
       </c>
@@ -4149,7 +4195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>47</v>
       </c>
@@ -4181,7 +4227,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>48</v>
       </c>
@@ -4216,7 +4262,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="57">
         <v>49</v>
       </c>
@@ -4248,7 +4294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>50</v>
       </c>
@@ -4280,7 +4326,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="57">
         <v>51</v>
       </c>
@@ -4312,7 +4358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>52</v>
       </c>
@@ -4344,7 +4390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>53</v>
       </c>
@@ -4376,7 +4422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="57">
         <v>54</v>
       </c>
@@ -4408,7 +4454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>55</v>
       </c>
@@ -4440,7 +4486,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="57">
         <v>56</v>
       </c>
@@ -4472,7 +4518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>57</v>
       </c>
@@ -4504,7 +4550,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>58</v>
       </c>
@@ -4536,7 +4582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="57">
         <v>59</v>
       </c>
@@ -4568,7 +4614,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>60</v>
       </c>
@@ -4613,14 +4659,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
@@ -4628,7 +4674,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>